<commit_message>
Adding 200 to Excel spreadsheet
Adding cell with 200 as an example
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -336,10 +336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -349,6 +349,11 @@
         <v>100</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes in branch 200
changes in branch 200 not clear
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -336,10 +336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -349,11 +349,6 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>200</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding 200 and 300
adding 200 and 300 to cells in spreadsheet
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -336,10 +336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -349,6 +349,16 @@
         <v>100</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>